<commit_message>
likert for end of camp
</commit_message>
<xml_diff>
--- a/Data/GGEE_23_END of CAMP Survey.xlsx
+++ b/Data/GGEE_23_END of CAMP Survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviarandell/Documents/GitHub/GGEESummer23/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007F09B9-3FE1-E64A-86BF-52595884E180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AAEE06-4D12-644D-9BFC-00D6B74FCC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="500" windowWidth="15600" windowHeight="16140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="500" windowWidth="15600" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cleaned Data 11_15" sheetId="1" r:id="rId1"/>
@@ -18306,8 +18306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C733FC2-ACE9-6F40-8491-D84751674D6A}">
   <dimension ref="A1:AG139"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="R1" sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -34095,8 +34095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6886F74B-AEFE-2D46-B5A4-3CD75EF45FC4}">
   <dimension ref="A1:AI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>